<commit_message>
process 2020 penetrom msmts
</commit_message>
<xml_diff>
--- a/data-raw/phen/rd_20200710-phen.xlsx
+++ b/data-raw/phen/rd_20200710-phen.xlsx
@@ -482,7 +482,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1150,7 @@
       <c r="H26" s="11">
         <v>13</v>
       </c>
-      <c r="I26" s="19" t="s">
+      <c r="J26" s="19" t="s">
         <v>21</v>
       </c>
       <c r="K26" s="15"/>

</xml_diff>